<commit_message>
Valores inseridos no Banco de Dados
</commit_message>
<xml_diff>
--- a/documentos/Backlog Requisitos (4).xlsx
+++ b/documentos/Backlog Requisitos (4).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/bruno_lima_sptech_school/Documents/git/sprint2/documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\sprint2\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{C04AB948-E61A-4C62-A176-3205C33EEB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2C23499-D59A-432E-9034-47CD6EA649AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454CC55A-C795-4187-9620-8411508DDD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -1002,10 +1002,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1322,34 +1318,34 @@
       <selection activeCell="B36" sqref="B36:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7265625" customWidth="1"/>
-    <col min="3" max="3" width="60.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="25"/>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26"/>
       <c r="C3" s="27"/>
       <c r="D3" s="28"/>
     </row>
-    <row r="4" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
     </row>
-    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1361,7 +1357,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1383,7 +1379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1427,14 +1423,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1445,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1456,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1467,7 +1463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1489,7 +1485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1500,7 +1496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1511,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1522,7 +1518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
@@ -1533,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1544,14 +1540,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1562,7 +1558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1573,7 +1569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
@@ -1584,14 +1580,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
@@ -1602,7 +1598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1613,7 +1609,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
@@ -1624,7 +1620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>54</v>
       </c>
@@ -1635,7 +1631,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>54</v>
       </c>
@@ -1646,7 +1642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
@@ -1657,7 +1653,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
@@ -1668,7 +1664,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>62</v>
       </c>
@@ -1679,7 +1675,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>64</v>
       </c>
@@ -1707,22 +1703,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7DA6DA-76F6-4BBF-B420-7F89428DFE23}">
   <dimension ref="B2:L54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="53.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.54296875" customWidth="1"/>
-    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1729,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -1742,7 +1738,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
     </row>
-    <row r="4" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +1749,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1776,7 +1772,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>70</v>
       </c>
@@ -1804,7 +1800,7 @@
       <c r="K6" s="32"/>
       <c r="L6" s="33"/>
     </row>
-    <row r="7" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>74</v>
       </c>
@@ -1836,7 +1832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>80</v>
       </c>
@@ -1871,7 +1867,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>82</v>
       </c>
@@ -1894,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
@@ -1919,7 +1915,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>136</v>
       </c>
@@ -1942,7 +1938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>88</v>
       </c>
@@ -1967,7 +1963,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1990,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>91</v>
       </c>
@@ -2013,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>93</v>
       </c>
@@ -2036,7 +2032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>96</v>
       </c>
@@ -2059,7 +2055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>99</v>
       </c>
@@ -2082,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>100</v>
       </c>
@@ -2107,7 +2103,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>102</v>
       </c>
@@ -2130,7 +2126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>104</v>
       </c>
@@ -2153,7 +2149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>106</v>
       </c>
@@ -2176,7 +2172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>108</v>
       </c>
@@ -2199,7 +2195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>110</v>
       </c>
@@ -2222,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>112</v>
       </c>
@@ -2245,7 +2241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>113</v>
       </c>
@@ -2268,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>117</v>
       </c>
@@ -2291,7 +2287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>119</v>
       </c>
@@ -2314,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>121</v>
       </c>
@@ -2337,7 +2333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>123</v>
       </c>
@@ -2360,7 +2356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>125</v>
       </c>
@@ -2383,7 +2379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
         <v>127</v>
       </c>
@@ -2406,7 +2402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>129</v>
       </c>
@@ -2429,7 +2425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>131</v>
       </c>
@@ -2452,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>132</v>
       </c>
@@ -2475,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>137</v>
       </c>
@@ -2486,19 +2482,19 @@
         <v>138</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="F35" s="11">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -2507,8 +2503,8 @@
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -2517,7 +2513,7 @@
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -2526,8 +2522,8 @@
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -2536,7 +2532,7 @@
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -2545,7 +2541,7 @@
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -2554,7 +2550,7 @@
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>

</xml_diff>